<commit_message>
Update ESTOQUE VG 12-02-2025.xlsx
</commit_message>
<xml_diff>
--- a/ESTOQUE VG 12-02-2025.xlsx
+++ b/ESTOQUE VG 12-02-2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos Eduardo\Documents\GitHub\App_Consulta_Veiculos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos Eduardo\Documents\GitHub\appiveco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7ADD44E-FAB3-47E1-9CCD-9A22D421418A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A248F20-B65C-42E9-A6FE-6E2794E4C03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{9D410868-8077-4D3C-BBE6-98234956D0C2}"/>
   </bookViews>
@@ -113,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +454,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +462,7 @@
     <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="115.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -476,10 +478,10 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
@@ -502,10 +504,10 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>2024</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>2024</v>
       </c>
       <c r="F2" t="s">
@@ -528,10 +530,10 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>2024</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>2024</v>
       </c>
       <c r="F3" t="s">

</xml_diff>